<commit_message>
Updated glycerol file in raw data to show animal ID
</commit_message>
<xml_diff>
--- a/data/raw/HFD vs Chow Glycerol Assay.xlsx
+++ b/data/raw/HFD vs Chow Glycerol Assay.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iharvey/Desktop/CushingAcromegalyStudy/data/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Exported" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -20,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="48">
   <si>
     <t>avg</t>
   </si>
@@ -162,6 +170,9 @@
   <si>
     <t>High Fat Diet</t>
   </si>
+  <si>
+    <t>ID</t>
+  </si>
 </sst>
 </file>
 
@@ -276,6 +287,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -380,11 +396,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2096218328"/>
-        <c:axId val="-2096215368"/>
+        <c:axId val="-755998032"/>
+        <c:axId val="-755880928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2096218328"/>
+        <c:axId val="-755998032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -394,12 +410,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096215368"/>
+        <c:crossAx val="-755880928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2096215368"/>
+        <c:axId val="-755880928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -409,7 +425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096218328"/>
+        <c:crossAx val="-755998032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -530,11 +546,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2106478056"/>
-        <c:axId val="-2114170424"/>
+        <c:axId val="-715372528"/>
+        <c:axId val="-715380704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2106478056"/>
+        <c:axId val="-715372528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,12 +560,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114170424"/>
+        <c:crossAx val="-715380704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2114170424"/>
+        <c:axId val="-715380704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106478056"/>
+        <c:crossAx val="-715372528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -719,20 +735,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114733864"/>
-        <c:axId val="-2114743672"/>
+        <c:axId val="-717939552"/>
+        <c:axId val="-713130240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114733864"/>
+        <c:axId val="-717939552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114743672"/>
+        <c:crossAx val="-713130240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -740,7 +757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114743672"/>
+        <c:axId val="-713130240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -750,7 +767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114733864"/>
+        <c:crossAx val="-717939552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -787,7 +804,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -910,20 +926,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2108721128"/>
-        <c:axId val="-2108718488"/>
+        <c:axId val="-713276784"/>
+        <c:axId val="-713279920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2108721128"/>
+        <c:axId val="-713276784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108718488"/>
+        <c:crossAx val="-713279920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -931,7 +948,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108718488"/>
+        <c:axId val="-713279920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,14 +958,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108721128"/>
+        <c:crossAx val="-713276784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1298,20 +1314,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114775816"/>
-        <c:axId val="-2114772792"/>
+        <c:axId val="-718130896"/>
+        <c:axId val="-718135056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114775816"/>
+        <c:axId val="-718130896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114772792"/>
+        <c:crossAx val="-718135056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1319,7 +1336,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114772792"/>
+        <c:axId val="-718135056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1330,7 +1347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114775816"/>
+        <c:crossAx val="-718130896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1341,7 +1358,6 @@
         <c:idx val="2"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1508,20 +1524,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2096175688"/>
-        <c:axId val="-2096172776"/>
+        <c:axId val="-713316080"/>
+        <c:axId val="-713330368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2096175688"/>
+        <c:axId val="-713316080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096172776"/>
+        <c:crossAx val="-713330368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1529,7 +1546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2096172776"/>
+        <c:axId val="-713330368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096175688"/>
+        <c:crossAx val="-713316080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2084,13 +2101,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S86"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F53" sqref="F18:H53"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1">
         <v>1</v>
       </c>
@@ -2116,7 +2133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2152,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.25</v>
       </c>
@@ -2188,7 +2205,7 @@
         <v>4.1999999999999996E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2.5</v>
       </c>
@@ -2216,7 +2233,7 @@
         <v>0.17249999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2252,7 +2269,7 @@
         <v>0.15650000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10</v>
       </c>
@@ -2282,7 +2299,7 @@
         <v>0.25800000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20</v>
       </c>
@@ -2314,7 +2331,7 @@
         <v>0.39750000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>3</v>
       </c>
@@ -2322,7 +2339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
         <v>4</v>
       </c>
@@ -2330,13 +2347,13 @@
         <v>2.41E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R16">
         <f>83/103</f>
         <v>0.80582524271844658</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -2380,7 +2397,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3035</v>
       </c>
@@ -2432,7 +2449,7 @@
         <v>0.84706387892948765</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3036</v>
       </c>
@@ -2484,7 +2501,7 @@
         <v>0.9195101317326676</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3037</v>
       </c>
@@ -2536,7 +2553,7 @@
         <v>1.0866937920476978</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3038</v>
       </c>
@@ -2588,7 +2605,7 @@
         <v>0.89721897702399678</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3039</v>
       </c>
@@ -2640,7 +2657,7 @@
         <v>0.73560810538613386</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3040</v>
       </c>
@@ -2692,7 +2709,7 @@
         <v>1.4433522673864294</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3041</v>
       </c>
@@ -2744,7 +2761,7 @@
         <v>0.75789926009480468</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3042</v>
       </c>
@@ -2811,7 +2828,7 @@
         <v>0.98568699727403364</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3048</v>
       </c>
@@ -2863,7 +2880,7 @@
         <v>0.36223126401589928</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3049</v>
       </c>
@@ -2915,7 +2932,7 @@
         <v>0.70774416200029544</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3050</v>
       </c>
@@ -2967,7 +2984,7 @@
         <v>0.42353193946474382</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3055</v>
       </c>
@@ -3019,7 +3036,7 @@
         <v>0.40681357343324076</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3056</v>
       </c>
@@ -3071,7 +3088,7 @@
         <v>0.80248156951214611</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3057</v>
       </c>
@@ -3123,7 +3140,7 @@
         <v>0.60743396581127718</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3058</v>
       </c>
@@ -3175,7 +3192,7 @@
         <v>0.65758906390578631</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3047</v>
       </c>
@@ -3242,7 +3259,7 @@
         <v>0.55031288187030847</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1747</v>
       </c>
@@ -3294,7 +3311,7 @@
         <v>0.91951013173266716</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1749</v>
       </c>
@@ -3346,7 +3363,7 @@
         <v>0.7801904148034754</v>
       </c>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1750</v>
       </c>
@@ -3398,7 +3415,7 @@
         <v>0.66316185258295413</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1766</v>
       </c>
@@ -3450,7 +3467,7 @@
         <v>0.58514281110260646</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1763</v>
       </c>
@@ -3502,7 +3519,7 @@
         <v>0.88607339966966125</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2102</v>
       </c>
@@ -3554,7 +3571,7 @@
         <v>0.85263666760665513</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2098</v>
       </c>
@@ -3606,7 +3623,7 @@
         <v>0.71331695067746326</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2099</v>
       </c>
@@ -3658,7 +3675,7 @@
         <v>0.98638359585867896</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2105</v>
       </c>
@@ -3710,7 +3727,7 @@
         <v>0.89721897702399678</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2107</v>
       </c>
@@ -3777,7 +3794,7 @@
         <v>0.80471068498301312</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1748</v>
       </c>
@@ -3829,7 +3846,7 @@
         <v>0.43467751681907912</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1751</v>
       </c>
@@ -3881,7 +3898,7 @@
         <v>1.025393116598853</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1745</v>
       </c>
@@ -3933,7 +3950,7 @@
         <v>1.4544978447407644</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1746</v>
       </c>
@@ -3985,7 +4002,7 @@
         <v>0.37337684137023464</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2108</v>
       </c>
@@ -4035,7 +4052,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2111</v>
       </c>
@@ -4087,7 +4104,7 @@
         <v>1.7331372785991488</v>
       </c>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2118</v>
       </c>
@@ -4137,7 +4154,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2123</v>
       </c>
@@ -4189,7 +4206,7 @@
         <v>0.65758906390578653</v>
       </c>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2127</v>
       </c>
@@ -4241,7 +4258,7 @@
         <v>0.79133599215781092</v>
       </c>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2128</v>
       </c>
@@ -4308,7 +4325,7 @@
         <v>0.89652237843935068</v>
       </c>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H57" t="s">
         <v>21</v>
       </c>
@@ -4322,7 +4339,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H58" t="s">
         <v>15</v>
       </c>
@@ -4341,7 +4358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H59" t="s">
         <v>16</v>
       </c>
@@ -4371,7 +4388,7 @@
         <v>1.1483187696883508E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H60" t="s">
         <v>17</v>
       </c>
@@ -4398,7 +4415,7 @@
         <v>0.61390878754420375</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="K61" t="s">
         <v>9</v>
       </c>
@@ -4411,12 +4428,12 @@
         <v>9.3565395042383745E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:19">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="O63" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:19">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H64" t="s">
         <v>18</v>
       </c>
@@ -4428,7 +4445,7 @@
         <v>8.432755255678645E-2</v>
       </c>
     </row>
-    <row r="65" spans="2:16">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
       <c r="H65" t="s">
         <v>19</v>
       </c>
@@ -4450,7 +4467,7 @@
         <v>8.7693382592572464E-2</v>
       </c>
     </row>
-    <row r="66" spans="2:16">
+    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
       <c r="H66" t="s">
         <v>20</v>
       </c>
@@ -4470,7 +4487,7 @@
         <v>8.56330686969832E-2</v>
       </c>
     </row>
-    <row r="67" spans="2:16">
+    <row r="67" spans="2:16" x14ac:dyDescent="0.2">
       <c r="K67" t="s">
         <v>11</v>
       </c>
@@ -4483,7 +4500,7 @@
         <v>5.8026524716456862E-2</v>
       </c>
     </row>
-    <row r="68" spans="2:16">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
       <c r="K68" t="s">
         <v>8</v>
       </c>
@@ -4496,7 +4513,7 @@
         <v>3.9799405550941198E-2</v>
       </c>
     </row>
-    <row r="69" spans="2:16">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
       <c r="K69" t="s">
         <v>9</v>
       </c>
@@ -4509,12 +4526,12 @@
         <v>0.15216421234595193</v>
       </c>
     </row>
-    <row r="73" spans="2:16">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.2">
       <c r="O73" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="2:16">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.2">
       <c r="N74" t="s">
         <v>10</v>
       </c>
@@ -4523,7 +4540,7 @@
         <v>0.98568699727403364</v>
       </c>
     </row>
-    <row r="75" spans="2:16">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D75" t="s">
         <v>31</v>
       </c>
@@ -4535,7 +4552,7 @@
         <v>0.55031288187030847</v>
       </c>
     </row>
-    <row r="76" spans="2:16">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>34</v>
       </c>
@@ -4547,7 +4564,7 @@
         <v>0.22648686030428763</v>
       </c>
     </row>
-    <row r="77" spans="2:16">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
         <v>33</v>
       </c>
@@ -4563,7 +4580,7 @@
         <v>0.80471068498301312</v>
       </c>
     </row>
-    <row r="78" spans="2:16">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.2">
       <c r="N78" t="s">
         <v>9</v>
       </c>
@@ -4572,7 +4589,7 @@
         <v>0.89652237843935068</v>
       </c>
     </row>
-    <row r="79" spans="2:16">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>35</v>
       </c>
@@ -4584,7 +4601,7 @@
         <v>0.36168741355463352</v>
       </c>
     </row>
-    <row r="80" spans="2:16">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
         <v>33</v>
       </c>
@@ -4593,7 +4610,7 @@
         <v>0.69571230982019361</v>
       </c>
     </row>
-    <row r="83" spans="2:4">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>34</v>
       </c>
@@ -4605,7 +4622,7 @@
         <v>0.22648686030428763</v>
       </c>
     </row>
-    <row r="84" spans="2:4">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
         <v>33</v>
       </c>
@@ -4614,7 +4631,7 @@
         <v>0.27489626556016594</v>
       </c>
     </row>
-    <row r="85" spans="2:4">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>35</v>
       </c>
@@ -4626,7 +4643,7 @@
         <v>0.36168741355463352</v>
       </c>
     </row>
-    <row r="86" spans="2:4">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
         <v>33</v>
       </c>
@@ -4639,473 +4656,574 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>3035</v>
+      </c>
+      <c r="B2">
         <f>Sheet1!F18</f>
         <v>0.20055325034578145</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>3036</v>
+      </c>
+      <c r="B3">
         <f>Sheet1!F19</f>
         <v>0.24896265560165967</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>3037</v>
+      </c>
+      <c r="B4">
         <f>Sheet1!F20</f>
         <v>0.22821576763485471</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>3038</v>
+      </c>
+      <c r="B5">
         <f>Sheet1!F21</f>
         <v>0.19363762102351312</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>3039</v>
+      </c>
+      <c r="B6">
         <f>Sheet1!F22</f>
         <v>0.28354080221300132</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>3040</v>
+      </c>
+      <c r="B7">
         <f>Sheet1!F23</f>
         <v>0.255878284923928</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>3041</v>
+      </c>
+      <c r="B8">
         <f>Sheet1!F24</f>
         <v>0.19363762102351312</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>3042</v>
+      </c>
+      <c r="B9">
         <f>Sheet1!F25</f>
         <v>0.2074688796680498</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>3048</v>
+      </c>
+      <c r="B10">
         <f>Sheet1!F26</f>
         <v>0.15214384508990311</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>3049</v>
+      </c>
+      <c r="B11">
         <f>Sheet1!F27</f>
         <v>0.31120331950207469</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>3050</v>
+      </c>
+      <c r="B12">
         <f>Sheet1!F28</f>
         <v>0.30428769017980634</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>3055</v>
+      </c>
+      <c r="B13">
         <f>Sheet1!F29</f>
         <v>0.22821576763485477</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>3056</v>
+      </c>
+      <c r="B14">
         <f>Sheet1!F30</f>
         <v>0.37344398340248969</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>44</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>3057</v>
+      </c>
+      <c r="B15">
         <f>Sheet1!F31</f>
         <v>0.33886583679114796</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>3058</v>
+      </c>
+      <c r="B16">
         <f>Sheet1!F32</f>
         <v>0.23513139695712312</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>3047</v>
+      </c>
+      <c r="B17">
         <f>Sheet1!F33</f>
         <v>0.255878284923928</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>1747</v>
+      </c>
+      <c r="B18">
         <f>Sheet1!F34</f>
         <v>0.43568464730290463</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
+        <v>1749</v>
+      </c>
+      <c r="B19">
         <f>Sheet1!F35</f>
         <v>0.24204702627939134</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>1750</v>
+      </c>
+      <c r="B20">
         <f>Sheet1!F36</f>
         <v>0.33195020746887965</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>43</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
+        <v>1766</v>
+      </c>
+      <c r="B21">
         <f>Sheet1!F37</f>
         <v>0.24896265560165967</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
+        <v>1763</v>
+      </c>
+      <c r="B22">
         <f>Sheet1!F38</f>
         <v>0.53941908713692943</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>43</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
+        <v>2102</v>
+      </c>
+      <c r="B23">
         <f>Sheet1!F39</f>
         <v>0.42185338865836797</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>43</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
+        <v>2098</v>
+      </c>
+      <c r="B24">
         <f>Sheet1!F40</f>
         <v>0.36652835408022133</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>43</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
+        <v>2099</v>
+      </c>
+      <c r="B25">
         <f>Sheet1!F41</f>
         <v>0.44951590594744134</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>43</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
+        <v>2105</v>
+      </c>
+      <c r="B26">
         <f>Sheet1!F42</f>
         <v>0.33195020746887965</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>43</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
+        <v>2107</v>
+      </c>
+      <c r="B27">
         <f>Sheet1!F43</f>
         <v>0.24896265560165967</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>43</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
+        <v>1748</v>
+      </c>
+      <c r="B28">
         <f>Sheet1!F44</f>
         <v>0.35269709543568467</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>44</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
+        <v>1751</v>
+      </c>
+      <c r="B29">
         <f>Sheet1!F45</f>
         <v>1.2517289073305671</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>44</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
+        <v>1745</v>
+      </c>
+      <c r="B30">
         <f>Sheet1!F46</f>
         <v>0.67081604426002761</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>44</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
+        <v>1746</v>
+      </c>
+      <c r="B31">
         <f>Sheet1!F47</f>
         <v>0.37344398340248969</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>44</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
+        <v>2108</v>
+      </c>
+      <c r="B32">
         <f>Sheet1!F48</f>
         <v>0.98893499308437083</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>44</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
+        <v>2111</v>
+      </c>
+      <c r="B33">
         <f>Sheet1!F49</f>
         <v>0.79529737206085749</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>44</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
+        <v>2118</v>
+      </c>
+      <c r="B34">
         <f>Sheet1!F50</f>
         <v>0.94052558782849249</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>44</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
+        <v>2123</v>
+      </c>
+      <c r="B35">
         <f>Sheet1!F51</f>
         <v>0.51867219917012453</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>44</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
+        <v>2127</v>
+      </c>
+      <c r="B36">
         <f>Sheet1!F52</f>
         <v>0.62240663900414928</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>44</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
+        <v>2128</v>
+      </c>
+      <c r="B37">
         <f>Sheet1!F53</f>
         <v>0.44260027662517304</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>44</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>